<commit_message>
fix item DB entry for mc_multiple
</commit_message>
<xml_diff>
--- a/documentation/example_surveys/all_widgets_with_values.xlsx
+++ b/documentation/example_surveys/all_widgets_with_values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -572,13 +572,6 @@
 What's your favourite TV series? If you need more choices (why would you), just add our own.</t>
   </si>
   <si>
-    <t>### check_button
-Like `check` with a larger button.
-This one has a skipIf: `confirm1 = 1`, so it will only be displayed if you checked that you wanted to be bothered with another question.  
-We can also use expressions like the one above to dynamically alter question text. For example, we can tell you that your preferred movies were `r all_widgets$m_fav_tv_series`.
-Skipifs can also refer to surveys that were answered before this one in the run.</t>
-  </si>
-  <si>
     <t>FALSE</t>
   </si>
   <si>
@@ -694,6 +687,13 @@
   </si>
   <si>
     <t>"The Wire"</t>
+  </si>
+  <si>
+    <t>### check_button
+Like `check` with a larger button.
+This one has a skipIf: `confirm1 = 1`, so it will only be displayed if you checked that you wanted to be bothered with another question.  
+We can also use expressions like the one above to dynamically alter question text. For example, we can tell you that your preferred movies were `r m_fav_tv_series`.
+Skipifs can also refer to surveys that were answered before this one in the run.</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1168,8 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M48" sqref="M48"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1224,7 +1224,7 @@
         <v>80</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="225">
@@ -1232,11 +1232,11 @@
         <v>142</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" s="3"/>
       <c r="G2" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="45">
@@ -1244,7 +1244,7 @@
         <v>142</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" s="3"/>
       <c r="G3" s="8" t="s">
@@ -1269,7 +1269,7 @@
         <v>103</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30">
@@ -1287,7 +1287,7 @@
         <v>100</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="105">
@@ -1298,11 +1298,11 @@
         <v>0</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E7" s="3"/>
       <c r="G7" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>20</v>
@@ -1311,7 +1311,7 @@
         <v>21</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="90">
@@ -1325,10 +1325,10 @@
         <v>85</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>30</v>
@@ -1337,7 +1337,7 @@
         <v>104</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="105">
@@ -1354,7 +1354,7 @@
         <v>145</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>42</v>
@@ -1363,7 +1363,7 @@
         <v>146</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60">
@@ -1374,7 +1374,7 @@
         <v>149</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>30</v>
@@ -1389,7 +1389,7 @@
         <v>114</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="75">
@@ -1397,10 +1397,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>30</v>
@@ -1409,7 +1409,7 @@
         <v>105</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="180">
@@ -1420,13 +1420,13 @@
         <v>139</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>106</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1443,7 +1443,7 @@
         <v>36</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>156</v>
@@ -1455,7 +1455,7 @@
         <v>109</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="45">
@@ -1463,13 +1463,13 @@
         <v>38</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>107</v>
@@ -1481,7 +1481,7 @@
         <v>111</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30">
@@ -1495,7 +1495,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>157</v>
@@ -1507,7 +1507,7 @@
         <v>112</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="30">
@@ -1518,13 +1518,13 @@
         <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>115</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="45">
@@ -1535,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>147</v>
@@ -1550,15 +1550,15 @@
         <v>15</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="30">
       <c r="A19" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="45">
@@ -1569,13 +1569,13 @@
         <v>23</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>116</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30">
@@ -1586,7 +1586,7 @@
         <v>24</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>168</v>
@@ -1598,7 +1598,7 @@
         <v>118</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30">
@@ -1609,7 +1609,7 @@
         <v>25</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>164</v>
@@ -1621,7 +1621,7 @@
         <v>135</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="45">
@@ -1632,29 +1632,29 @@
         <v>26</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>133</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30">
       <c r="E24" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30">
       <c r="E25" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="34">
@@ -1663,10 +1663,10 @@
       </c>
       <c r="B26" s="12"/>
       <c r="E26" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="30">
@@ -1677,13 +1677,13 @@
         <v>16</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>119</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="45">
@@ -1694,13 +1694,13 @@
         <v>9</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>120</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1714,13 +1714,13 @@
         <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>121</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1731,13 +1731,13 @@
         <v>52</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>53</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1748,13 +1748,13 @@
         <v>46</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>43</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1765,13 +1765,13 @@
         <v>47</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>56</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1782,19 +1782,19 @@
         <v>49</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>50</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="E35" s="3"/>
       <c r="M35" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="45">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="E36" s="3"/>
       <c r="M36" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="75">
@@ -1814,13 +1814,13 @@
         <v>70</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>165</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30">
@@ -1831,13 +1831,13 @@
         <v>75</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>166</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -1848,13 +1848,13 @@
         <v>74</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>71</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30">
@@ -1865,21 +1865,21 @@
         <v>136</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>58</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30">
       <c r="E41" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M41" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="45">
@@ -1890,13 +1890,13 @@
         <v>59</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>159</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30">
@@ -1907,13 +1907,13 @@
         <v>61</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>122</v>
       </c>
       <c r="M43" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30">
@@ -1924,13 +1924,13 @@
         <v>63</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>64</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="45">
@@ -1941,21 +1941,21 @@
         <v>90</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>123</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30">
       <c r="E46" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="45">
@@ -1966,7 +1966,7 @@
         <v>65</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>170</v>
@@ -1975,7 +1975,7 @@
         <v>66</v>
       </c>
       <c r="M47" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="45">
@@ -1986,7 +1986,7 @@
         <v>67</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>169</v>
@@ -1995,22 +1995,22 @@
         <v>66</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="2:13" ht="30">
       <c r="E49" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="2:13" ht="30">
       <c r="E50" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="2:13" ht="30">
       <c r="E51" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="2:13" ht="30">
@@ -2022,7 +2022,7 @@
         <v>137</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="4" t="s">
@@ -2034,7 +2034,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="2:13" ht="60">
@@ -2048,11 +2048,11 @@
         <v>138</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>127</v>
@@ -2070,7 +2070,7 @@
         <v>131</v>
       </c>
       <c r="M53" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="2:13" ht="45">
@@ -2084,7 +2084,7 @@
         <v>94</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
@@ -2106,7 +2106,7 @@
         <v>131</v>
       </c>
       <c r="M54" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="2:13" ht="45">
@@ -2120,7 +2120,7 @@
         <v>95</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3" t="s">
@@ -2142,79 +2142,79 @@
         <v>131</v>
       </c>
       <c r="M55" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="2:13" ht="30">
       <c r="B56" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>167</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3" t="s">
         <v>125</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J56" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L56" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="K56" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L56" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="M56" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="57" spans="2:13" ht="30">
       <c r="B57" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>167</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3" t="s">
         <v>126</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J57" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L57" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="K57" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L57" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="M57" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="2:13">
@@ -2229,7 +2229,7 @@
         <v>132</v>
       </c>
       <c r="M58" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="2:13" ht="195">
@@ -2243,10 +2243,10 @@
         <v>161</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
       <c r="M59" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
don't let show if, dynamic value fail silently
</commit_message>
<xml_diff>
--- a/documentation/example_surveys/all_widgets_with_values.xlsx
+++ b/documentation/example_surveys/all_widgets_with_values.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="209">
   <si>
     <t>mc</t>
   </si>
@@ -638,9 +638,6 @@
 Click Cthulhu to show the other items!</t>
   </si>
   <si>
-    <t>bla@example.com</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -650,25 +647,13 @@
     <t>0</t>
   </si>
   <si>
-    <t>11:01</t>
-  </si>
-  <si>
-    <t>29.04.1989</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
     <t>911</t>
   </si>
   <si>
-    <t>http://formr.org</t>
-  </si>
-  <si>
     <t>200</t>
-  </si>
-  <si>
-    <t>#ff00ff</t>
   </si>
   <si>
     <t>mc_button1</t>
@@ -694,6 +679,24 @@
 This one has a skipIf: `confirm1 = 1`, so it will only be displayed if you checked that you wanted to be bothered with another question.  
 We can also use expressions like the one above to dynamically alter question text. For example, we can tell you that your preferred movies were `r m_fav_tv_series`.
 Skipifs can also refer to surveys that were answered before this one in the run.</t>
+  </si>
+  <si>
+    <t>"http://formr.org"</t>
+  </si>
+  <si>
+    <t>"11:01"</t>
+  </si>
+  <si>
+    <t>"bla@example.com"</t>
+  </si>
+  <si>
+    <t>"#ff00ff"</t>
+  </si>
+  <si>
+    <t>"2012-02-01"</t>
+  </si>
+  <si>
+    <t>"Europe - Berlin"</t>
   </si>
 </sst>
 </file>
@@ -820,7 +823,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="9" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1168,8 +1171,8 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1409,7 +1412,7 @@
         <v>105</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="180">
@@ -1426,7 +1429,7 @@
         <v>106</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1555,7 +1558,7 @@
     </row>
     <row r="19" spans="1:13" ht="30">
       <c r="A19" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>184</v>
@@ -1638,7 +1641,7 @@
         <v>133</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30">
@@ -1682,8 +1685,8 @@
       <c r="G27" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="M27" s="9" t="s">
-        <v>194</v>
+      <c r="M27" s="13" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="45">
@@ -1699,8 +1702,8 @@
       <c r="G28" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="M28" s="9" t="s">
-        <v>195</v>
+      <c r="M28" s="13" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1720,7 +1723,7 @@
         <v>121</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1820,7 +1823,7 @@
         <v>165</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30">
@@ -1837,7 +1840,7 @@
         <v>166</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -1854,7 +1857,7 @@
         <v>71</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30">
@@ -1870,8 +1873,8 @@
       <c r="G40" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="M40" s="9" t="s">
-        <v>200</v>
+      <c r="M40" s="13" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30">
@@ -1975,7 +1978,7 @@
         <v>66</v>
       </c>
       <c r="M47" s="9" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="45">
@@ -1995,7 +1998,7 @@
         <v>66</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="2:13" ht="30">
@@ -2033,8 +2036,8 @@
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
-      <c r="M52" s="9" t="s">
-        <v>182</v>
+      <c r="M52" s="13" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="2:13" ht="60">
@@ -2147,13 +2150,13 @@
     </row>
     <row r="56" spans="2:13" ht="30">
       <c r="B56" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>167</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>184</v>
@@ -2169,27 +2172,27 @@
         <v>186</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M56" s="9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="2:13" ht="30">
       <c r="B57" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>167</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>184</v>
@@ -2205,16 +2208,16 @@
         <v>186</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M57" s="9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58" spans="2:13">
@@ -2243,7 +2246,7 @@
         <v>161</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="M59" s="9" t="s">
         <v>182</v>
@@ -2252,8 +2255,8 @@
   </sheetData>
   <autoFilter ref="G42:G45"/>
   <hyperlinks>
-    <hyperlink ref="M11" r:id="rId1"/>
-    <hyperlink ref="M38" r:id="rId2"/>
+    <hyperlink ref="M11" r:id="rId1" display="bla@example.com"/>
+    <hyperlink ref="M38" r:id="rId2" display="http://formr.org"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>